<commit_message>
Minor Changes has been pushed
</commit_message>
<xml_diff>
--- a/target/test-classes/TestCases.xlsx
+++ b/target/test-classes/TestCases.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\eclipse-workspace\testng\ecommerce\src\test\resources\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="109">
   <si>
     <t>testEcommerceWebsite</t>
   </si>
@@ -401,7 +401,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -493,35 +492,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -815,22 +786,22 @@
   <dimension ref="A2:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.54296875"/>
-    <col min="3" max="3" customWidth="true" width="20.6328125"/>
-    <col min="4" max="4" customWidth="true" width="17.453125"/>
-    <col min="5" max="5" customWidth="true" width="22.81640625"/>
-    <col min="6" max="6" customWidth="true" width="21.36328125"/>
-    <col min="7" max="7" customWidth="true" width="18.08984375"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.81640625"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="11.54296875"/>
-    <col min="10" max="10" customWidth="true" width="12.36328125"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="7.36328125"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="9.81640625"/>
+    <col min="2" max="2" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6328125" customWidth="1"/>
+    <col min="4" max="4" width="17.453125" customWidth="1"/>
+    <col min="5" max="5" width="22.81640625" customWidth="1"/>
+    <col min="6" max="6" width="21.36328125" customWidth="1"/>
+    <col min="7" max="7" width="18.08984375" customWidth="1"/>
+    <col min="8" max="8" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.36328125" customWidth="1"/>
+    <col min="11" max="11" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1353,7 +1324,7 @@
       </c>
       <c r="I20" s="7"/>
       <c r="J20" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K20" s="8" t="s">
         <v>27</v>
@@ -1387,7 +1358,7 @@
       </c>
       <c r="I21" s="7"/>
       <c r="J21" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K21" s="8" t="s">
         <v>27</v>
@@ -1421,7 +1392,7 @@
       </c>
       <c r="I22" s="7"/>
       <c r="J22" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K22" s="8" t="s">
         <v>27</v>
@@ -1455,7 +1426,7 @@
       </c>
       <c r="I23" s="7"/>
       <c r="J23" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K23" s="8" t="s">
         <v>27</v>
@@ -1489,7 +1460,7 @@
       </c>
       <c r="I24" s="7"/>
       <c r="J24" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K24" s="8" t="s">
         <v>27</v>
@@ -1523,7 +1494,7 @@
       </c>
       <c r="I25" s="7"/>
       <c r="J25" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K25" s="8" t="s">
         <v>27</v>
@@ -1620,17 +1591,17 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>107</v>
       </c>
     </row>

</xml_diff>